<commit_message>
optimized headshot name matching + fix for complex last names
</commit_message>
<xml_diff>
--- a/data/website_data.xlsx
+++ b/data/website_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arvindmurugan/Library/CloudStorage/Dropbox/GDrive/GDrive Work Files/Murugan Website/2025 Faculty UChicago Website Claude/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arvindmurugan/Library/CloudStorage/Dropbox/GDrive/GDrive Work Files/Murugan Website/2025 GitHub Faculty Website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7500CB-BA0C-B344-A1AC-39DF7BDAB496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F8D523-481C-BD48-B74A-A1D2C45E8883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talks" sheetId="1" r:id="rId1"/>
@@ -1390,9 +1390,6 @@
     <t>LaNijah</t>
   </si>
   <si>
-    <t>O’Brien</t>
-  </si>
-  <si>
     <t>Jackson</t>
   </si>
   <si>
@@ -1968,6 +1965,9 @@
   <si>
     <t>Many observations about the surprising uniformity of the large scale structure of the universe is explained by cosmic inflation. In this model, a "ball" (the inflaton) gently rolls down a smooth hill, causing rapid expansion of the universe in size. But what is this "ball" and what is the hill it is running down? We built a mechanistic model of inflation based on string theory, with different membrane-like objects (D3 and D7 branes) and their interactions playing the role of the ball and the hill.  We computed what the shape of the hill would be from this mechanistic theory for cosmic inflation which has consequences for experimental signatures of inflation (e.g., in the cosmic microwave background).</t>
   </si>
+  <si>
+    <t>OBrien</t>
+  </si>
 </sst>
 </file>
 
@@ -1975,7 +1975,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -2120,7 +2120,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -4856,7 +4856,7 @@
   </sheetPr>
   <dimension ref="A1:AA1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8522,9 +8522,9 @@
   </sheetPr>
   <dimension ref="A1:AD1009"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8943,10 +8943,10 @@
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="11" t="s">
+        <v>643</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>454</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>455</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>383</v>
@@ -8962,7 +8962,7 @@
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="18" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
@@ -8971,10 +8971,10 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>457</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>458</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>383</v>
@@ -8990,7 +8990,7 @@
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="18" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
@@ -8999,10 +8999,10 @@
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>460</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>461</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>383</v>
@@ -9017,24 +9017,24 @@
         <v>13</v>
       </c>
       <c r="G19" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="H19" s="10" t="s">
         <v>462</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>463</v>
       </c>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>465</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>466</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>383</v>
@@ -9050,21 +9050,21 @@
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" s="18" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>469</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>470</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>383</v>
@@ -9080,7 +9080,7 @@
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="18" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
@@ -9089,10 +9089,10 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>472</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>473</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>383</v>
@@ -9110,7 +9110,7 @@
         <v>415</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
@@ -9118,10 +9118,10 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="11" t="s">
+        <v>474</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>475</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>476</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>383</v>
@@ -9132,10 +9132,10 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>477</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>478</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>386</v>
@@ -9150,10 +9150,10 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>479</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>480</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>386</v>
@@ -9168,10 +9168,10 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>481</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>482</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>386</v>
@@ -9187,15 +9187,15 @@
       </c>
       <c r="G26" s="5"/>
       <c r="I26" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>484</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>485</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>386</v>
@@ -9210,10 +9210,10 @@
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>486</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>487</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>386</v>
@@ -9231,10 +9231,10 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>488</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>489</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>386</v>
@@ -9252,10 +9252,10 @@
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>490</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>491</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>386</v>
@@ -9268,15 +9268,15 @@
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>493</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>494</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>386</v>
@@ -9289,15 +9289,15 @@
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="18" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>496</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>497</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>386</v>
@@ -9310,15 +9310,15 @@
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="18" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>499</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>500</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>386</v>
@@ -9331,15 +9331,15 @@
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>502</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>503</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>386</v>
@@ -9352,15 +9352,15 @@
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>505</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>506</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>386</v>
@@ -9373,18 +9373,18 @@
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="K35" s="18" t="s">
         <v>507</v>
-      </c>
-      <c r="K35" s="18" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>509</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>510</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>386</v>
@@ -9397,15 +9397,15 @@
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>386</v>
@@ -9418,15 +9418,15 @@
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>515</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>516</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>386</v>
@@ -9439,18 +9439,18 @@
       </c>
       <c r="G38" s="5"/>
       <c r="H38" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="K38" s="5" t="s">
         <v>517</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>386</v>
@@ -9463,18 +9463,18 @@
       </c>
       <c r="G39" s="5"/>
       <c r="H39" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>520</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>521</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>386</v>
@@ -9487,7 +9487,7 @@
       </c>
       <c r="G40" s="5"/>
       <c r="H40" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12419,15 +12419,15 @@
         <v>330</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>524</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>525</v>
       </c>
       <c r="D2" s="5"/>
     </row>
@@ -12439,10 +12439,10 @@
         <v>326</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>526</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12453,10 +12453,10 @@
         <v>326</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>528</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12467,10 +12467,10 @@
         <v>326</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>530</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12481,10 +12481,10 @@
         <v>326</v>
       </c>
       <c r="C6" s="21" t="s">
+        <v>531</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>532</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12495,10 +12495,10 @@
         <v>326</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>534</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12506,13 +12506,13 @@
         <v>45453</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>536</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>526</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -12557,21 +12557,21 @@
         <v>321</v>
       </c>
       <c r="C1" s="19" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>538</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>540</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>541</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>542</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>281</v>
@@ -12579,13 +12579,13 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>544</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>281</v>
@@ -12593,13 +12593,13 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>546</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>547</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>156</v>
@@ -12607,13 +12607,13 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>548</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>549</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>550</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>261</v>
@@ -12621,16 +12621,16 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>551</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>552</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>553</v>
       </c>
     </row>
   </sheetData>
@@ -12658,25 +12658,25 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="19" t="s">
+        <v>553</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>554</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>556</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>557</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>558</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>559</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>560</v>
       </c>
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
@@ -12703,10 +12703,10 @@
         <v>324</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>561</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>562</v>
       </c>
       <c r="D2" s="5">
         <v>2024</v>
@@ -12715,10 +12715,10 @@
         <v>325</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>563</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12726,10 +12726,10 @@
         <v>322</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>565</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>566</v>
       </c>
       <c r="D3" s="5">
         <v>2025</v>
@@ -12738,33 +12738,33 @@
         <v>323</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>568</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>569</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>570</v>
       </c>
       <c r="D4" s="5">
         <v>2025</v>
       </c>
       <c r="E4" s="12" t="s">
+        <v>570</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>572</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12772,22 +12772,22 @@
         <v>327</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>574</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>575</v>
       </c>
       <c r="D5" s="5">
         <v>2024</v>
       </c>
       <c r="E5" s="12" t="s">
+        <v>575</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>577</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12795,275 +12795,275 @@
         <v>328</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>579</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>580</v>
       </c>
       <c r="D6" s="5">
         <v>2023</v>
       </c>
       <c r="E6" s="12" t="s">
+        <v>580</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>581</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>583</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>584</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>585</v>
       </c>
       <c r="D7" s="5">
         <v>2022</v>
       </c>
       <c r="E7" s="12" t="s">
+        <v>585</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>586</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>588</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>589</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>590</v>
       </c>
       <c r="D8" s="5">
         <v>2023</v>
       </c>
       <c r="E8" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>591</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>593</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>594</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D9" s="5">
         <v>2022</v>
       </c>
       <c r="E9" s="12" t="s">
+        <v>594</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>595</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>577</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>597</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>598</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>599</v>
       </c>
       <c r="D10" s="5">
         <v>2021</v>
       </c>
       <c r="E10" s="12" t="s">
+        <v>599</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>600</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>563</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
+        <v>601</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>602</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>603</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>604</v>
       </c>
       <c r="D11" s="5">
         <v>2021</v>
       </c>
       <c r="E11" s="12" t="s">
+        <v>604</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>605</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>607</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>608</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>609</v>
       </c>
       <c r="D12" s="5">
         <v>2021</v>
       </c>
       <c r="E12" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>610</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>563</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>612</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>613</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>614</v>
       </c>
       <c r="D13" s="5">
         <v>2020</v>
       </c>
       <c r="E13" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>615</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>617</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>618</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>619</v>
       </c>
       <c r="D14" s="5">
         <v>2017</v>
       </c>
       <c r="E14" s="12" t="s">
+        <v>619</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>620</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>623</v>
-      </c>
       <c r="C15" s="5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D15" s="5">
         <v>2014</v>
       </c>
       <c r="E15" s="12" t="s">
+        <v>623</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>624</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
+        <v>625</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>627</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>628</v>
       </c>
       <c r="D16" s="5">
         <v>2014</v>
       </c>
       <c r="E16" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>629</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>563</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D17" s="5">
         <v>2012</v>
       </c>
       <c r="E17" s="12" t="s">
+        <v>631</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>632</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>563</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13071,45 +13071,45 @@
         <v>316</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>634</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>635</v>
       </c>
       <c r="D18" s="5">
         <v>2008</v>
       </c>
       <c r="E18" s="12" t="s">
+        <v>635</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>637</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>640</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>641</v>
       </c>
       <c r="D19" s="5">
         <v>2006</v>
       </c>
       <c r="E19" s="21" t="s">
+        <v>641</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>642</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>637</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>